<commit_message>
Test_Cases with Hardware and software validation
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Test_Cases_V_2.0.xlsx
+++ b/Documents/Second_Week/Test_Cases_V_2.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project Managment\DDM\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project Managment\DDM\Documents\Second_Week\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="154">
   <si>
     <t>ID</t>
   </si>
@@ -620,6 +620,137 @@
   </si>
   <si>
     <t>TC3.12</t>
+  </si>
+  <si>
+    <t>TC4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- LCD 2*16 is available.
+2- Atmega 32 is available.
+3- 5 volt battary.
+</t>
+  </si>
+  <si>
+    <t>Validate connection of LCD to Atmega32 when make orderusing Atmega to light all leds in LCD</t>
+  </si>
+  <si>
+    <t>All leds in LCD should be lighten.</t>
+  </si>
+  <si>
+    <t>1- Connect pin VSS in LCD to ground.
+2- Connect pin VCC in LCD to 5V battery.
+3- Connect pin VEE in LCD to Resistance 10K then the other leg of the resistance to the ground.
+4- Connect RS pin in LCD to PC0 in ATmega32.
+5- Connect RW pin in LCD to PC1 in ATmega32.
+6- Connect E pin in LCD to PC2 in ATmega32.
+7- Connect PD0 in LCD to pin PB0 in Atmega32.
+8- Connect PD1 in LCD to pin PB1 in Atmega32.
+9- Connect PD2 in LCD to pin PB2 in Atmega32.
+10- Connect PD3 in LCD to pin PB3 in Atmega32.
+11- Connect PD4 in LCD to pin PB4 in Atmega32.
+12- Connect PD5 in LCD to pin PB5 in Atmega32.
+13- Connect PD6 in LCD to pin PB6 in Atmega32.
+14- Connect PD7 in LCD to pin PB7 in Atmega32.
+15- Connect VCC in Atmega32 to 5Volt battarey.
+16- Connect GND pin in Atmega32 to Ground.
+17- make code with software to light all Leds of the LCD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate connection of Ultra sonic to Atmega32 and the LCD when make order using Atmega to Measure the distance </t>
+  </si>
+  <si>
+    <t>1- Connect pin VSS in LCD to ground.
+2- Connect pin VCC in LCD to 5V battery.
+3- Connect pin VEE in LCD to Resistance 10K then the other leg of the resistance to the ground.
+4- Connect RS pin in LCD to PC0 in ATmega32.
+5- Connect RW pin in LCD to PC1 in ATmega32.
+6- Connect E pin in LCD to PC2 in ATmega32.
+7- Connect PD0 in LCD to pin PB0 in Atmega32.
+8- Connect PD1 in LCD to pin PB1 in Atmega32.
+9- Connect PD2 in LCD to pin PB2 in Atmega32.
+10- Connect PD3 in LCD to pin PB3 in Atmega32.
+11- Connect PD4 in LCD to pin PB4 in Atmega32.
+12- Connect PD5 in LCD to pin PB5 in Atmega32.
+13- Connect PD6 in LCD to pin PB6 in Atmega32.
+14- Connect PD7 in LCD to pin PB7 in Atmega32.
+15- Connect VCC in Atmega32 to 5Volt battarey.
+16- Connect GND pin in Atmega32 to Ground.
+17- Connect treg pin in ultrasonic to PA0 in Atmega32.
+18- Connect echo pin in ultrasonic to PD6 in Atmega32.
+19- Connect VCC pin in ultrasonic to 5 volt.
+20- Connect GND pin in ultrasonic to Ground.
+21- make code with software to test the sensor by displaying reading of distance in LCD.
+22- make an object facing the ultrasonic with less than 300cm and more than 2 cm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the readings should be displayed in LCD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Hardware </t>
+  </si>
+  <si>
+    <t>TC4.1</t>
+  </si>
+  <si>
+    <t>Validate Software</t>
+  </si>
+  <si>
+    <t>1- Connect pin VSS in LCD to ground.
+2- Connect pin VCC in LCD to 5V battery.
+3- Connect pin VEE in LCD to Resistance 10K then the other leg of the resistance to the ground.
+4- Connect RS pin in LCD to PC0 in ATmega32.
+5- Connect RW pin in LCD to PC1 in ATmega32.
+6- Connect E pin in LCD to PC2 in ATmega32.
+7- Connect PD0 in LCD to pin PB0 in Atmega32.
+8- Connect PD1 in LCD to pin PB1 in Atmega32.
+9- Connect PD2 in LCD to pin PB2 in Atmega32.
+10- Connect PD3 in LCD to pin PB3 in Atmega32.
+11- Connect PD4 in LCD to pin PB4 in Atmega32.
+12- Connect PD5 in LCD to pin PB5 in Atmega32.
+13- Connect PD6 in LCD to pin PB6 in Atmega32.
+14- Connect PD7 in LCD to pin PB7 in Atmega32.
+15- Connect VCC in Atmega32 to 5Volt battarey.
+16- Connect GND pin in Atmega32 to Ground.
+17- Connect treg pin in ultrasonic to PA0 in Atmega32.
+18- Connect echo pin in ultrasonic to PD6 in Atmega32.
+19- Connect VCC pin in ultrasonic to 5 volt.
+20- Connect GND pin in ultrasonic to Ground.
+21- Configure echo pin in ultrasonic as input pin.
+22- Configure trig pin in ultrasonic as output pin.
+23- make code with software to test the sensor by displaying reading of distance in LCD.
+22- make an object facing the ultrasonic with less than 300cm and more than 2 cm.</t>
+  </si>
+  <si>
+    <t>Validate configuration of echo and trig pins in Ultrasonic sensor</t>
+  </si>
+  <si>
+    <t>1- Connect pin VSS in LCD to ground.
+2- Connect pin VCC in LCD to 5V battery.
+3- Connect pin VEE in LCD to Resistance 10K then the other leg of the resistance to the ground.
+4- Connect RS pin in LCD to PC0 in ATmega32.
+5- Connect RW pin in LCD to PC1 in ATmega32.
+6- Connect E pin in LCD to PC2 in ATmega32.
+7- Connect PD0 in LCD to pin PB0 in Atmega32.
+8- Connect PD1 in LCD to pin PB1 in Atmega32.
+9- Connect PD2 in LCD to pin PB2 in Atmega32.
+10- Connect PD3 in LCD to pin PB3 in Atmega32.
+11- Connect PD4 in LCD to pin PB4 in Atmega32.
+12- Connect PD5 in LCD to pin PB5 in Atmega32.
+13- Connect PD6 in LCD to pin PB6 in Atmega32.
+14- Connect PD7 in LCD to pin PB7 in Atmega32.
+15- Connect VCC in Atmega32 to 5Volt battarey.
+16- Connect GND pin in Atmega32 to Ground.
+17- Connect treg pin in ultrasonic to PA0 in Atmega32.
+18- Connect echo pin in ultrasonic to PD6 in Atmega32.
+19- Connect VCC pin in ultrasonic to 5 volt.
+20- Connect GND pin in ultrasonic to Ground.
+21- Configure echo pin in ultrasonic as output pin.
+22- Configure trig pin in ultrasonic as input pin.
+23- make code with software to test the sensor by displaying reading of distance in LCD.
+24- make an object facing the ultrasonic with less than 300cm and more than 2 cm.</t>
+  </si>
+  <si>
+    <t>No reading displayed in LCD.</t>
   </si>
 </sst>
 </file>
@@ -1107,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,6 +2306,136 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>4</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>4</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="15" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>